<commit_message>
created and reviewed the test cases for my account for enter vpn and created test cases for symlex settings(general)
</commit_message>
<xml_diff>
--- a/apps/features/backlog/android/auto_connect_settings.xlsx
+++ b/apps/features/backlog/android/auto_connect_settings.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\backlog\android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C1697B-2C65-4884-BEAF-CA70D6DB002D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0221D1-314C-4DD2-9D02-32E092C3A81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="General Settings (Settings)" sheetId="1" r:id="rId1"/>
+    <sheet name="Auto Connect (Settings)" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -46,95 +46,14 @@
     <t>*****</t>
   </si>
   <si>
+    <t>TC_SYM_STAC_001</t>
+  </si>
+  <si>
     <t>1.The Symlex VPN app is installed and configured on the Android device.
 2. The user is logged in to the VPN app.</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>TC_SYM_GST_001</t>
-  </si>
-  <si>
-    <t>TC_SYM_GST_002</t>
-  </si>
-  <si>
-    <t>TC_SYM_GST_003</t>
-  </si>
-  <si>
-    <t>TC_SYM_GST_004</t>
-  </si>
-  <si>
-    <t>TC_SYM_GST_005</t>
-  </si>
-  <si>
-    <t>TC_SYM_GST_006</t>
-  </si>
-  <si>
-    <t>TC_SYM_GST_007</t>
-  </si>
-  <si>
-    <t>TC_SYM_GST_008</t>
-  </si>
-  <si>
-    <t>Verify General Settings Expansion</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Verify Collapse of General Settings</t>
-  </si>
-  <si>
-    <t>Verify Options in Expanded  General Settings</t>
-  </si>
-  <si>
-    <t>Verify Default Selection of General Setting Options</t>
-  </si>
-  <si>
-    <t>Verify Quick Access Button Functionality</t>
-  </si>
-  <si>
-    <t>Verify Quick Access with Inactive VPN</t>
-  </si>
-  <si>
-    <t>Verify always selected server  Button Functionality</t>
-  </si>
-  <si>
-    <t>Verify Always selected server with Inactive VPN</t>
-  </si>
-  <si>
-    <t>1. Go to Playstore and install SymlexVPN in the mobile.
-2. Open the installed SymlexVPN Application.
-3. Input Password to the password field
-4. Tap on login button
-5. Disconnect the VPN 
-6. Navigate to the "Always selected server" section..
-7. Click on the "Always selected server" button.</t>
-  </si>
-  <si>
-    <t>The user should be selected to the default or last-used server but No attempt to establish a VPN connection should be made.</t>
-  </si>
-  <si>
-    <t>The user should be connected to the default or last-used server.</t>
-  </si>
-  <si>
-    <t>1. Go to Playstore and install SymlexVPN in the mobile.
-2. Open the installed SymlexVPN Application.
-3. Input Password to the password field
-4. Tap on login button
-5. Navigate to the "General Settings" section..
-6. Locate the "Always selected server" button on the main screen.
-7. Click on the "Always selected server" button.</t>
-  </si>
-  <si>
-    <t>1. Go to Playstore and install SymlexVPN in the mobile.
-2. Open the installed SymlexVPN Application.
-3. Input Password to the password field
-4. Tap on login button
-5. Disconnect the VPN 
-6. Navigate to the "General Settings" section..
-7. Click on the "Quick Access" button.</t>
-  </si>
-  <si>
-    <t>Scenario : General Settings (Settings)</t>
+    <t>Verify Auto Connect Expansion</t>
   </si>
   <si>
     <t>1. Go to Playstore and install SymlexVPN in the mobile.
@@ -142,54 +61,141 @@
 3. Input Password to the password field
 4. Tap on login button
 5. Connect the VPN 
-6. Navigate to the "General Settings" section..
-7. Check if there is an option to expand the general settings.</t>
+6. Navigate to the "Auto Connect" section.
+7. Check if there is an option to expand theAuto Connect</t>
   </si>
   <si>
-    <t xml:space="preserve">The general settings should have an expandable section,  indicating that it can be expanded </t>
+    <t>The Auto Connect should have an expandable section,  indicating that it can be expanded</t>
   </si>
   <si>
-    <t>The general settings section should collapse, hiding additional options.</t>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>TC_SYM_STAC_002</t>
+  </si>
+  <si>
+    <t>TC_SYM_STAC_003</t>
+  </si>
+  <si>
+    <t>TC_SYM_STAC_004</t>
+  </si>
+  <si>
+    <t>TC_SYM_STAC_005</t>
+  </si>
+  <si>
+    <t>TC_SYM_STAC_006</t>
+  </si>
+  <si>
+    <t>TC_SYM_STAC_007</t>
+  </si>
+  <si>
+    <t>TC_SYM_STAC_008</t>
+  </si>
+  <si>
+    <t>TC_SYM_STAC_009</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify Collapse of Auto Connect</t>
   </si>
   <si>
     <t>1. Go to Playstore and install SymlexVPN in the mobile.
 2. Open the installed SymlexVPN Application.
 3. Input Password to the password field
 4. Tap on login button
-5. Navigate to the "General Settings" section..
-6. Verify that the general settings are initially expanded.
+5. Navigate to the "Auto Connect" section.
+6. Verify that the Auto Connect are initially expanded.
 7. Click on the collapse icon or text.</t>
+  </si>
+  <si>
+    <t>The auto connect section should collapse, hiding additional options.</t>
+  </si>
+  <si>
+    <t>Verify Options in Expanded Auto Connect</t>
   </si>
   <si>
     <t>1. Go to Playstore and install SymlexVPN in the mobile.
 2. Open the installed SymlexVPN Application.
 3. Input Password to the password field
 4. Tap on login button
-5. Navigate to the "General Settings" section..
-6. Verify the presence of options like "Quick Access" and "Always Select Server" in the expanded section.</t>
+5. Navigate to the "Auto Connect" section..
+6. Verify the presence of options like "OFF" and "ON" in the expanded section.</t>
   </si>
   <si>
-    <t>The expanded general settings should display the options "Quick Access" and "Always Select Server."</t>
+    <t>The expanded auto connect should display the options "off" and "on."</t>
   </si>
   <si>
-    <t>as a default selection " Always select server" will show</t>
+    <t>Verify Default Selection of Auto Connect Options</t>
   </si>
   <si>
     <t>1. Go to Playstore and install SymlexVPN in the mobile.
 2. Open the installed SymlexVPN Application.
 3. Input Password to the password field
 4. Tap on login button
-5. Navigate to the "General Settings" section..
-6. Locate the "Quick Access" button on the main screen.
-7. Click on the "Quick Access" button.</t>
+5. Navigate to the "Auto Connect" section..
+6. Check if the default selection for options like "OFF" or "ON" is as expected.</t>
+  </si>
+  <si>
+    <t>as a default selection "OFF" will show</t>
+  </si>
+  <si>
+    <t>Enable Auto Connect Without VPN connection</t>
   </si>
   <si>
     <t>1. Go to Playstore and install SymlexVPN in the mobile.
 2. Open the installed SymlexVPN Application.
 3. Input Password to the password field
 4. Tap on login button
-5. Navigate to the "General Settings" section..
-6. Check if the default selection for options like "Quick Access" or "Always Select Server" is as expected.</t>
+5. Navigate to the "Auto Connect" section..
+6. Click on the "ON" button.</t>
+  </si>
+  <si>
+    <t>The VPN will connect automatically.</t>
+  </si>
+  <si>
+    <t>Enable Auto Connect with VPN connection</t>
+  </si>
+  <si>
+    <t>Verify auto connection without internet</t>
+  </si>
+  <si>
+    <t>1. Go to Playstore and install SymlexVPN in the mobile.
+2. Open the installed SymlexVPN Application.
+3. Input Password to the password field
+4. Tap on login button
+5. turn off the internet
+6. Navigate to the "Auto connect" section of settings
+7. Click on the "ON" button.</t>
+  </si>
+  <si>
+    <t>The VPN will not connect automatically and should show an error message " No internet connection. pleasse check your internet"</t>
+  </si>
+  <si>
+    <t>Disable Auto Connect with VPN</t>
+  </si>
+  <si>
+    <t>1. Go to Playstore and install SymlexVPN in the mobile.
+2. Open the installed SymlexVPN Application.
+3. Input Password to the password field
+4. Tap on login button
+5. Navigate to the "Auto connect" section of settings
+6. Click on the "off" button.</t>
+  </si>
+  <si>
+    <t>The VPN will not connect automatically.</t>
+  </si>
+  <si>
+    <t>Disable Auto Connect without  VPN</t>
+  </si>
+  <si>
+    <t>1. Go to Playstore and install SymlexVPN in the mobile.
+2. Open the installed SymlexVPN Application.
+3. Input Password to the password field
+4. Tap on login button
+5. Navigate to the "Auto connect" section of settings
+7. Click on the "off" button.</t>
+  </si>
+  <si>
+    <t>Scenario : Auto Connect (Settings)</t>
   </si>
 </sst>
 </file>
@@ -380,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -404,11 +410,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -431,11 +448,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1138,8 +1150,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1155,15 +1167,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>31</v>
+      <c r="A1" s="24" t="s">
+        <v>43</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="19"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="10"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1185,13 +1197,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1255,25 +1267,25 @@
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>8</v>
+      <c r="D4" s="14" t="s">
+        <v>11</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>18</v>
+      <c r="E4" s="14" t="s">
+        <v>12</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>32</v>
+      <c r="F4" s="14" t="s">
+        <v>13</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="14" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="5"/>
@@ -1297,23 +1309,23 @@
       <c r="Z4" s="5"/>
     </row>
     <row r="5" spans="1:26" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>11</v>
+      <c r="A5" s="14" t="s">
+        <v>14</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>8</v>
+      <c r="B5" s="14" t="s">
+        <v>9</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>19</v>
+      <c r="C5" s="20" t="s">
+        <v>22</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>35</v>
+      <c r="D5" s="20" t="s">
+        <v>23</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>34</v>
+      <c r="E5" s="20" t="s">
+        <v>24</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>9</v>
+      <c r="F5" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="5"/>
@@ -1337,23 +1349,23 @@
       <c r="Z5" s="5"/>
     </row>
     <row r="6" spans="1:26" ht="108" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>12</v>
+      <c r="A6" s="14" t="s">
+        <v>15</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>8</v>
+      <c r="B6" s="14" t="s">
+        <v>9</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>20</v>
+      <c r="C6" s="20" t="s">
+        <v>25</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>36</v>
+      <c r="D6" s="20" t="s">
+        <v>26</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>37</v>
+      <c r="E6" s="20" t="s">
+        <v>27</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>9</v>
+      <c r="F6" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="5"/>
@@ -1377,23 +1389,23 @@
       <c r="Z6" s="5"/>
     </row>
     <row r="7" spans="1:26" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="5"/>
@@ -1417,25 +1429,25 @@
       <c r="Z7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>14</v>
+      <c r="A8" s="14" t="s">
+        <v>17</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="9" t="s">
+      <c r="B8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="11"/>
+      <c r="C8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="18"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -1456,26 +1468,26 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>15</v>
+    <row r="9" spans="1:26" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>18</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="B9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="12"/>
+      <c r="C9" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="19"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -1496,26 +1508,26 @@
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
     </row>
-    <row r="10" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>16</v>
+    <row r="10" spans="1:26" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>19</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="9" t="s">
+      <c r="B10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="C10" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="19"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
@@ -1536,26 +1548,26 @@
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
     </row>
-    <row r="11" spans="1:26" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>17</v>
+    <row r="11" spans="1:26" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>20</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="9" t="s">
+      <c r="B11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="10"/>
+      <c r="C11" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="16"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1577,15 +1589,25 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="9" t="s">
+      <c r="A12" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="10"/>
+      <c r="C12" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="16"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>

</xml_diff>